<commit_message>
Updated Framework 2.0 - 10 July 2024
</commit_message>
<xml_diff>
--- a/error_log_report/failed_cases.xlsx
+++ b/error_log_report/failed_cases.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sitegen" sheetId="1" r:id="rId1"/>
-    <sheet name="TOTP" sheetId="2" r:id="rId2"/>
-    <sheet name="TORA" sheetId="3" r:id="rId3"/>
+    <sheet name="Medical" sheetId="1" r:id="rId1"/>
+    <sheet name="Abbvie" sheetId="2" r:id="rId2"/>
+    <sheet name="ADPA" sheetId="3" r:id="rId3"/>
     <sheet name="AMI" sheetId="4" r:id="rId4"/>
-    <sheet name="Allerganpro" sheetId="5" r:id="rId5"/>
-    <sheet name="ADPA" sheetId="6" r:id="rId6"/>
-    <sheet name="Abbvie" sheetId="7" r:id="rId7"/>
-    <sheet name="Abbvie Pro Medical" sheetId="8" r:id="rId8"/>
+    <sheet name="Sitegen" sheetId="5" r:id="rId5"/>
+    <sheet name="TORA" sheetId="6" r:id="rId6"/>
+    <sheet name="Allerganpro" sheetId="7" r:id="rId7"/>
+    <sheet name="TOTP" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -420,104 +420,142 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Demo</v>
+        <v>Central East Europe</v>
       </c>
       <c r="B2" t="str">
-        <v>https://demo-preview.abbviepro.com</v>
+        <v>https://medical-preview.abbviepro.com/cee/ro.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T11:11:23.304Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T09:48:44.914Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Hoidontueksi</v>
+        <v>Germany</v>
       </c>
       <c r="B3" t="str">
-        <v>https://preview.hoidontueksi.fi</v>
+        <v>https://medical-preview.abbviepro.com/de/de.html</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T11:11:34.980Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T09:48:45.072Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Kestavaterveydenhuolto</v>
+        <v>Sweden</v>
       </c>
       <c r="B4" t="str">
-        <v>https://preview.kestavaterveydenhuolto.fi/</v>
+        <v>https://medical-preview.abbviepro.com/se/sv.html</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T11:11:41.441Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T09:49:13.404Z</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>test</v>
+        <v>Denmark</v>
       </c>
       <c r="B5" t="str">
-        <v>https://preview.test-hcv.nl/</v>
+        <v>https://medical-preview.abbviepro.com/dk/da.html</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
-</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-06-13T11:11:41.626Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D5">
+        <v>404</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-07-10T09:49:21.164Z</v>
       </c>
     </row>
     <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>Beroerteherstel</v>
+        <v>Norway</v>
       </c>
       <c r="B6" t="str">
-        <v>https://preview.beroerteherstel.nl</v>
+        <v>https://medical-preview.abbviepro.com/no/no.html</v>
       </c>
       <c r="C6" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
-</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2024-06-13T11:11:53.677Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2024-07-10T09:49:21.556Z</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7" t="str">
+        <v>Ireland</v>
+      </c>
+      <c r="B7" t="str">
+        <v>https://medical-preview.abbviepro.com/ie/en.html</v>
+      </c>
+      <c r="C7" t="str" xml:space="preserve">
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D7">
+        <v>404</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2024-07-10T09:50:54.805Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -533,87 +571,82 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>France</v>
+        <v>North West Africa</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preview.taleoftwopatients.com/fr/fr.html</v>
+        <v>https://preview.abbviepro.com/nwa/en.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T11:19:47.898Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T09:56:27.167Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>United Kingdom</v>
+        <v>Croatia</v>
       </c>
       <c r="B3" t="str">
-        <v>https://preview.taleoftwopatients.com/gb/en.html</v>
+        <v>https://preview.abbviepro.com/si/produodopa-calculator.html</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T11:19:48.079Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T09:57:18.317Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Deutschland</v>
+        <v>Training</v>
       </c>
       <c r="B4" t="str">
-        <v>https://preview.taleoftwopatients.com/de/de.html</v>
+        <v>https://training-preview.abbviepro.com</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T11:19:48.183Z</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>Mexico</v>
-      </c>
-      <c r="B5" t="str">
-        <v>https://preview.taleoftwopatients.com/mx/es.html</v>
-      </c>
-      <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-06-13T11:19:48.674Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T09:57:36.258Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -629,87 +662,82 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Japan</v>
+        <v>France</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preview.talkoverra.com/jp/ja.html</v>
+        <v>https://preview.lets-talk-eczema.com/fr/fr.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T11:41:20.233Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T09:58:13.422Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Slovakia</v>
+        <v>Austria</v>
       </c>
       <c r="B3" t="str">
-        <v>https://preview.talkoverra.com/sk/sk.html</v>
+        <v>https://preview.lets-talk-eczema.com/ca/en.html</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T11:41:52.952Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T09:58:44.357Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Romania</v>
+        <v>Gulf</v>
       </c>
       <c r="B4" t="str">
-        <v>https://preview.talkoverra.com/ro/ro.html</v>
+        <v>https://preview.lets-talk-eczema.com/gu/en.html</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T11:41:56.921Z</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>Turkey</v>
-      </c>
-      <c r="B5" t="str">
-        <v>https://preview.talkoverra.com/tr/tr.html</v>
-      </c>
-      <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-06-13T11:41:58.878Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T09:59:24.032Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -725,6 +753,9 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
@@ -781,20 +812,23 @@
 _x001b_[2m  -   unexpected value ""_x001b_[22m
 </v>
       </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T12:08:32.683Z</v>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T09:59:55.405Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -810,36 +844,182 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>India</v>
+        <v>Support Center</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preview.allerganpro.com/in/en.html</v>
+        <v>https://help-preview.abbviepro.com</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T12:21:20.351Z</v>
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T10:00:55.304Z</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Demo</v>
+      </c>
+      <c r="B3" t="str">
+        <v>https://demo-preview.abbviepro.com</v>
+      </c>
+      <c r="C3" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T10:01:01.765Z</v>
+      </c>
+    </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>Hoidontueksi</v>
+      </c>
+      <c r="B4" t="str">
+        <v>https://preview.hoidontueksi.fi</v>
+      </c>
+      <c r="C4" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T10:01:12.590Z</v>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5" t="str">
+        <v>test</v>
+      </c>
+      <c r="B5" t="str">
+        <v>https://preview.test-hcv.nl/</v>
+      </c>
+      <c r="C5" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D5">
+        <v>404</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-07-10T10:01:33.161Z</v>
+      </c>
+    </row>
+    <row r="6" xml:space="preserve">
+      <c r="A6" t="str">
+        <v>Kestavaterveydenhuolto</v>
+      </c>
+      <c r="B6" t="str">
+        <v>https://preview.kestavaterveydenhuolto.fi/</v>
+      </c>
+      <c r="C6" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D6">
+        <v>404</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2024-07-10T10:01:35.715Z</v>
+      </c>
+    </row>
+    <row r="7" xml:space="preserve">
+      <c r="A7" t="str">
+        <v>Beroerteherstel</v>
+      </c>
+      <c r="B7" t="str">
+        <v>https://preview.beroerteherstel.nl</v>
+      </c>
+      <c r="C7" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D7">
+        <v>404</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2024-07-10T10:01:50.069Z</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8" t="str">
+        <v>Vyalev</v>
+      </c>
+      <c r="B8" t="str">
+        <v>https://preview.vyalev.com.au/</v>
+      </c>
+      <c r="C8" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D8">
+        <v>404</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2024-07-10T10:02:01.524Z</v>
+      </c>
+    </row>
+    <row r="9" xml:space="preserve">
+      <c r="A9" t="str">
+        <v>Aquipta</v>
+      </c>
+      <c r="B9" t="str">
+        <v>https://preview.aquipta.co.nz/</v>
+      </c>
+      <c r="C9" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.waitForSelector: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]') to be visible_x001b_[22m
+</v>
+      </c>
+      <c r="D9">
+        <v>404</v>
+      </c>
+      <c r="E9" t="str">
+        <v>2024-07-10T10:02:02.270Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -855,70 +1035,102 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>France</v>
+        <v>Japan</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preview.lets-talk-eczema.com/fr/fr.html</v>
+        <v>https://preview.talkoverra.com/jp/ja.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: net::ERR_SSL_VERSION_OR_CIPHER_MISMATCH at https://preview.lets-talk-eczema.com/fr/fr.html
-Call log:
-  _x001b_[2m- navigating to "https://preview.lets-talk-eczema.com/fr/fr.html", waiting until "load"_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T12:29:50.000Z</v>
+        <v xml:space="preserve">page.fill: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T10:02:27.840Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Austria</v>
+        <v>Turkey</v>
       </c>
       <c r="B3" t="str">
-        <v>https://preview.lets-talk-eczema.com/ca/en.html</v>
+        <v>https://preview.talkoverra.com/tr/tr.html</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T12:37:03.695Z</v>
+        <v xml:space="preserve">page.fill: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T10:02:49.285Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Gulf</v>
+        <v>Slovakia</v>
       </c>
       <c r="B4" t="str">
-        <v>https://preview.lets-talk-eczema.com/gu/en.html</v>
+        <v>https://preview.talkoverra.com/sk/sk.html</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T12:37:10.049Z</v>
+        <v xml:space="preserve">page.fill: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T10:02:51.121Z</v>
+      </c>
+    </row>
+    <row r="5" xml:space="preserve">
+      <c r="A5" t="str">
+        <v>Romania</v>
+      </c>
+      <c r="B5" t="str">
+        <v>https://preview.talkoverra.com/ro/ro.html</v>
+      </c>
+      <c r="C5" t="str" xml:space="preserve">
+        <v xml:space="preserve">page.fill: Timeout 10000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D5">
+        <v>404</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-07-10T10:03:07.964Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -934,87 +1146,42 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Canada</v>
+        <v>India</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preview.abbviepro.com/ca/en.html</v>
+        <v>https://preview.allerganpro.com/in/en.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.goto: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- navigating to "https://preview.abbviepro.com/ca/en.html", waiting until "load"_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T12:50:42.349Z</v>
-      </c>
-    </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
-        <v>North West Africa</v>
-      </c>
-      <c r="B3" t="str">
-        <v>https://preview.abbviepro.com/nwa/en.html</v>
-      </c>
-      <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T12:51:12.360Z</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
-        <v>Croatia</v>
-      </c>
-      <c r="B4" t="str">
-        <v>https://preview.abbviepro.com/si/produodopa-calculator.html</v>
-      </c>
-      <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T12:52:07.631Z</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>Training</v>
-      </c>
-      <c r="B5" t="str">
-        <v>https://training-preview.abbviepro.com</v>
-      </c>
-      <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-06-13T12:52:24.994Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T10:03:20.634Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1030,97 +1197,95 @@
         <v>errorMessage</v>
       </c>
       <c r="D1" t="str">
+        <v>statusCode</v>
+      </c>
+      <c r="E1" t="str">
         <v>timestamp</v>
       </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Central East Europe</v>
+        <v>United Kingdom</v>
       </c>
       <c r="B2" t="str">
-        <v>https://medical-preview.abbviepro.com/cee/ro.html</v>
+        <v>https://preview.taleoftwopatients.com/gb/en.html</v>
       </c>
       <c r="C2" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2024-06-13T13:00:24.861Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D2">
+        <v>404</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2024-07-10T10:06:49.257Z</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Sweden</v>
+        <v>France</v>
       </c>
       <c r="B3" t="str">
-        <v>https://medical-preview.abbviepro.com/se/sv.html</v>
+        <v>https://preview.taleoftwopatients.com/fr/fr.html</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2024-06-13T13:00:48.995Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D3">
+        <v>404</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2024-07-10T10:06:49.334Z</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Denmark</v>
+        <v>Mexico</v>
       </c>
       <c r="B4" t="str">
-        <v>https://medical-preview.abbviepro.com/dk/da.html</v>
+        <v>https://preview.taleoftwopatients.com/mx/es.html</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2024-06-13T13:00:53.602Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D4">
+        <v>404</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2024-07-10T10:06:51.180Z</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>Norway</v>
+        <v>Deutschland</v>
       </c>
       <c r="B5" t="str">
-        <v>https://medical-preview.abbviepro.com/no/no.html</v>
+        <v>https://preview.taleoftwopatients.com/de/de.html</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2024-06-13T13:01:00.787Z</v>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6" t="str">
-        <v>Ireland</v>
-      </c>
-      <c r="B6" t="str">
-        <v>https://medical-preview.abbviepro.com/ie/en.html</v>
-      </c>
-      <c r="C6" t="str" xml:space="preserve">
-        <v xml:space="preserve">page.fill: Test timeout of 440000ms exceeded.
-Call log:
-  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
-</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2024-06-13T13:02:29.269Z</v>
+        <v xml:space="preserve">Login failed: page.fill: Test timeout of 240000ms exceeded.
+Call log:
+  _x001b_[2m- waiting for locator('input[name="username"]')_x001b_[22m
+</v>
+      </c>
+      <c r="D5">
+        <v>404</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2024-07-10T10:06:53.112Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>